<commit_message>
Fix combiner in Ahom
</commit_message>
<xml_diff>
--- a/py_convert/ONE_DATA/Oneida_spreadsheet.xlsx
+++ b/py_convert/ONE_DATA/Oneida_spreadsheet.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,16 +21,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <r>
-      <rPr>
-        <sz val="20"/>
-        <rFont val="Oneida"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ukwehok&amp;</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Uk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">w</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">eh</t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="true"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">k&amp;</t>
     </r>
     <r>
       <rPr>
@@ -41,6 +81,44 @@
       </rPr>
       <t xml:space="preserve">ha</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SUPER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sub</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Yukhinulh@ ohw^tsya&gt;</t>
@@ -58,9 +136,10 @@
     <r>
       <rPr>
         <u val="single"/>
-        <sz val="16"/>
-        <rFont val="Oneida"/>
-        <family val="1"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ha</t>
     </r>
@@ -87,9 +166,10 @@
     <r>
       <rPr>
         <u val="single"/>
-        <sz val="16"/>
-        <rFont val="Oneida"/>
-        <family val="1"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e</t>
     </r>
@@ -119,6 +199,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e&gt;</t>
     </r>
@@ -148,6 +229,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">w#</t>
     </r>
@@ -177,6 +259,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">le&gt;</t>
     </r>
@@ -195,6 +278,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">u</t>
     </r>
@@ -224,6 +308,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ha</t>
     </r>
@@ -244,6 +329,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ha</t>
     </r>
@@ -262,6 +348,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e</t>
     </r>
@@ -291,6 +378,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e</t>
     </r>
@@ -320,6 +408,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e</t>
     </r>
@@ -349,6 +438,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ha</t>
     </r>
@@ -378,6 +468,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ha</t>
     </r>
@@ -407,6 +498,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ha</t>
     </r>
@@ -436,6 +528,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e&gt;</t>
     </r>
@@ -465,6 +558,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e&gt;</t>
     </r>
@@ -494,6 +588,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e&gt;</t>
     </r>
@@ -514,6 +609,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&amp;=</t>
     </r>
@@ -543,6 +639,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e</t>
     </r>
@@ -561,6 +658,7 @@
         <sz val="16"/>
         <rFont val="Oneida"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">e&gt;</t>
     </r>
@@ -579,6 +677,151 @@
   </si>
   <si>
     <t xml:space="preserve">Shukwaya&gt;t$su (n#= olihwakwe=k&amp; lawy&lt;n&lt;t@=u)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duplicate of line 18</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="32"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Shukwaya&gt;t$</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="32"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">su</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="32"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (n#= olihwakwe=k&amp; lawy&lt;n&lt;t@=u)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Copy of line 21, but with underline added.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sheet2 Uk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">w</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">eh</t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="true"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">o</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">k&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SUP</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <vertAlign val="superscript"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ER&gt;^</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="20"/>
+        <rFont val="Oneida"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sub&lt;&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -588,11 +831,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -610,6 +854,27 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="20"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="20"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="20"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
       <sz val="20"/>
       <name val="Oneida"/>
       <family val="0"/>
@@ -623,10 +888,78 @@
       <charset val="1"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
+      <sz val="20"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="20"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="20"/>
+      <name val="Oneida"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <u val="single"/>
       <sz val="16"/>
       <name val="Oneida"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="32"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="20"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="32"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <vertAlign val="superscript"/>
+      <sz val="20"/>
+      <name val="Oneida"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -671,7 +1004,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -682,6 +1015,30 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -701,10 +1058,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -714,11 +1071,11 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -866,20 +1223,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+    <row r="21" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="72" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -891,4 +1267,37 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="119.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="50.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>